<commit_message>
Weekly Orchestration - 2025-05-19
</commit_message>
<xml_diff>
--- a/reports/portfolio-2025-05-16.xlsx
+++ b/reports/portfolio-2025-05-16.xlsx
@@ -922,7 +922,7 @@
         <v>0.4</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.4158935206504775</v>
+        <v>0.4158935206504772</v>
       </c>
       <c r="BE2" t="n">
         <v>0.342721222779036</v>
@@ -1303,7 +1303,7 @@
         <v>0.01</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.09999999999999973</v>
+        <v>0.09999999999999989</v>
       </c>
       <c r="BD4" t="n">
         <v>0.1958913831738001</v>
@@ -1498,13 +1498,13 @@
         <v>0.05000000000000002</v>
       </c>
       <c r="BD5" t="n">
-        <v>0.1773978570947949</v>
+        <v>0.1773978570947952</v>
       </c>
       <c r="BE5" t="n">
         <v>0.2236353566260657</v>
       </c>
       <c r="BF5" t="n">
-        <v>0.7932460223247115</v>
+        <v>0.7932460223247125</v>
       </c>
     </row>
     <row r="6">
@@ -1687,16 +1687,16 @@
         <v>0.01</v>
       </c>
       <c r="BC6" t="n">
-        <v>0.05000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="BD6" t="n">
-        <v>0.1803764500168985</v>
+        <v>0.1803764500168987</v>
       </c>
       <c r="BE6" t="n">
         <v>0.2269068959430459</v>
       </c>
       <c r="BF6" t="n">
-        <v>0.7949359549750016</v>
+        <v>0.7949359549750026</v>
       </c>
     </row>
   </sheetData>
@@ -40317,7 +40317,7 @@
         <v>0.1786</v>
       </c>
       <c r="U2" t="n">
-        <v>-0.1073418972697711</v>
+        <v>-0.1073418972697708</v>
       </c>
       <c r="V2" t="n">
         <v>0.1622550010394427</v>
@@ -40587,7 +40587,7 @@
         <v>0.1287</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.07803615570751266</v>
+        <v>-0.07803615570751254</v>
       </c>
       <c r="V5" t="n">
         <v>0.1285355331005558</v>
@@ -40684,42 +40684,42 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>LQD</t>
+          <t>IGOV</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>iShares iBoxx $ Investment Grade Corporate Bond ETF</t>
+          <t>iShares International Treasury Bond ETF</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2.22%</t>
+          <t>8.65%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>7.50%</t>
+          <t>9.56%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2.61%</t>
+          <t>-0.71%</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>-0.17%</t>
+          <t>-3.32%</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2.37%</t>
+          <t>-0.86%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>4.41%</t>
+          <t>0.21%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -40729,87 +40729,87 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Jul 22, 2002</t>
+          <t>Jan 21, 2009</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>29697566053</v>
+        <v>976165647</v>
       </c>
       <c r="L7" t="n">
-        <v>239566</v>
+        <v>239830</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>https://www.blackrock.com/us/individual/products/239566/ishares-iboxx-investment-grade-corporate-bond-etf</t>
+          <t>https://www.blackrock.com/us/individual/products/239830/ishares-international-treasury-bond-etf</t>
         </is>
       </c>
       <c r="N7" t="n">
-        <v>0.054</v>
+        <v>0.029</v>
       </c>
       <c r="O7" t="n">
-        <v>12.82</v>
+        <v>9.59</v>
       </c>
       <c r="P7" t="n">
         <v>1.11</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.044</v>
+        <v>0.022</v>
       </c>
       <c r="R7" t="n">
-        <v>90.748</v>
+        <v>94.584</v>
       </c>
       <c r="S7" t="n">
-        <v>9.74</v>
+        <v>8.531000000000001</v>
       </c>
       <c r="T7" t="n">
-        <v>0.0974</v>
+        <v>0.0853</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.007895941115029115</v>
+        <v>-0.04012984225208993</v>
       </c>
       <c r="V7" t="n">
-        <v>0.08775496924607881</v>
+        <v>0.0962651767413395</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>IGOV</t>
+          <t>LQD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>iShares International Treasury Bond ETF</t>
+          <t>iShares iBoxx $ Investment Grade Corporate Bond ETF</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>8.65%</t>
+          <t>2.22%</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>9.56%</t>
+          <t>7.50%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-0.71%</t>
+          <t>2.61%</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-3.32%</t>
+          <t>-0.17%</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>-0.86%</t>
+          <t>2.37%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.21%</t>
+          <t>4.41%</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -40819,46 +40819,46 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Jan 21, 2009</t>
+          <t>Jul 22, 2002</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>976165647</v>
+        <v>29697566053</v>
       </c>
       <c r="L8" t="n">
-        <v>239830</v>
+        <v>239566</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>https://www.blackrock.com/us/individual/products/239830/ishares-international-treasury-bond-etf</t>
+          <t>https://www.blackrock.com/us/individual/products/239566/ishares-iboxx-investment-grade-corporate-bond-etf</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>0.029</v>
+        <v>0.054</v>
       </c>
       <c r="O8" t="n">
-        <v>9.59</v>
+        <v>12.82</v>
       </c>
       <c r="P8" t="n">
         <v>1.11</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.022</v>
+        <v>0.044</v>
       </c>
       <c r="R8" t="n">
-        <v>94.584</v>
+        <v>90.748</v>
       </c>
       <c r="S8" t="n">
-        <v>8.531000000000001</v>
+        <v>9.74</v>
       </c>
       <c r="T8" t="n">
-        <v>0.0853</v>
+        <v>0.0974</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.04012984225208993</v>
+        <v>-0.007895941115029115</v>
       </c>
       <c r="V8" t="n">
-        <v>0.0962651767413395</v>
+        <v>0.08775496924607881</v>
       </c>
     </row>
     <row r="9">
@@ -41022,22 +41022,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.008119256878070294</v>
+        <v>0.008119256878070297</v>
       </c>
       <c r="D2" t="n">
-        <v>0.911234433708664</v>
+        <v>0.9112344337086636</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5460232349157121</v>
+        <v>0.546023234915712</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2981413730678191</v>
+        <v>0.2981413730678187</v>
       </c>
       <c r="G2" t="n">
-        <v>7.71062401169841e-06</v>
+        <v>7.710624011698427e-06</v>
       </c>
       <c r="H2" t="n">
-        <v>0.253025158580136</v>
+        <v>0.2530251585801359</v>
       </c>
     </row>
     <row r="3">
@@ -41055,19 +41055,19 @@
         <v>0.02484299227788999</v>
       </c>
       <c r="D3" t="n">
-        <v>1.389678712204903</v>
+        <v>1.389678712204901</v>
       </c>
       <c r="E3" t="n">
         <v>0.5297559219006347</v>
       </c>
       <c r="F3" t="n">
-        <v>0.280641336788791</v>
+        <v>0.2806413367887912</v>
       </c>
       <c r="G3" t="n">
-        <v>1.598670324787288e-05</v>
+        <v>1.5986703247873e-05</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03039607086740378</v>
+        <v>0.03039607086740376</v>
       </c>
     </row>
     <row r="4">
@@ -41082,22 +41082,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.007026719569467179</v>
+        <v>0.007026719569467176</v>
       </c>
       <c r="D4" t="n">
         <v>1.108788422010107</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6789105477693995</v>
+        <v>0.6789105477693994</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4609195318725464</v>
+        <v>0.4609195318725465</v>
       </c>
       <c r="G4" t="n">
-        <v>3.421215591521256e-09</v>
+        <v>3.421215591521207e-09</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2488001377030982</v>
+        <v>0.2488001377030984</v>
       </c>
     </row>
     <row r="5">
@@ -41112,22 +41112,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.01799706731455273</v>
+        <v>0.01799706731455272</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5341939692771701</v>
+        <v>0.5341939692771699</v>
       </c>
       <c r="E5" t="n">
         <v>0.3246387433906265</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1053903137102449</v>
+        <v>0.105390313710245</v>
       </c>
       <c r="G5" t="n">
         <v>0.01212128798145995</v>
       </c>
       <c r="H5" t="n">
-        <v>0.02517503420392517</v>
+        <v>0.02517503420392522</v>
       </c>
     </row>
     <row r="6">
@@ -41145,19 +41145,19 @@
         <v>0.01063177962568217</v>
       </c>
       <c r="D6" t="n">
-        <v>1.053515437448797</v>
+        <v>1.053515437448796</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6286338878588601</v>
+        <v>0.6286338878588604</v>
       </c>
       <c r="F6" t="n">
-        <v>0.395180564964546</v>
+        <v>0.3951805649645462</v>
       </c>
       <c r="G6" t="n">
         <v>9.758831530800996e-08</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1103210587501004</v>
+        <v>0.1103210587501003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>